<commit_message>
count3:schedule CD4 lab appoitment form update
</commit_message>
<xml_diff>
--- a/config/forms/app/count.xlsx
+++ b/config/forms/app/count.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="65">
   <si>
     <t>type</t>
   </si>
@@ -138,20 +138,45 @@
     <t>today()</t>
   </si>
   <si>
+    <t>select_one due</t>
+  </si>
+  <si>
+    <t>duee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This patient is due for a CD4 count. 
+</t>
+  </si>
+  <si>
     <t>list_name</t>
   </si>
   <si>
-    <t>unsuppressed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unsuppressed (CD4 count is below 350 cells/mm3)
+    <t>unstable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unstable (CD4 count is below 350 cells/mm3)
 </t>
   </si>
   <si>
-    <t>suppressed</t>
-  </si>
-  <si>
-    <t>Suppressed (CD4 count is 350 or above 350 cells/mm3)</t>
+    <t>stable</t>
+  </si>
+  <si>
+    <t>Stable (CD4 count is 350 or above 350 cells/mm3)</t>
+  </si>
+  <si>
+    <t>due</t>
+  </si>
+  <si>
+    <t>due1</t>
+  </si>
+  <si>
+    <t>Okay, I will, schedule an appointment for a lab visit</t>
+  </si>
+  <si>
+    <t>due2</t>
+  </si>
+  <si>
+    <t>Snooze task for 2 days</t>
   </si>
   <si>
     <t>form_title</t>
@@ -173,6 +198,9 @@
   </si>
   <si>
     <t>default_language</t>
+  </si>
+  <si>
+    <t>Schedule CD4 Lab Appointment</t>
   </si>
   <si>
     <t>pages</t>
@@ -541,6 +569,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
+    <col customWidth="1" min="1" max="1" width="20.0"/>
     <col customWidth="1" min="3" max="3" width="30.0"/>
   </cols>
   <sheetData>
@@ -890,7 +919,20 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="9" t="s">
         <v>27</v>
       </c>
     </row>
@@ -914,7 +956,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -927,22 +969,44 @@
       <c r="A2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>43</v>
+      <c r="B2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>45</v>
+      <c r="B3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -959,50 +1023,53 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="30.75"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="12" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C2" s="13" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-06-29_23-41</v>
+        <v>2022-07-11_14-21</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="14" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>